<commit_message>
vault backup: 2022-11-10 12:33:31
</commit_message>
<xml_diff>
--- a/情感识别论文统计.xlsx
+++ b/情感识别论文统计.xlsx
@@ -8,17 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F143EF71-1E59-489B-98A4-A22BEA263044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA277412-2972-43CD-B248-C12330EEB26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1104" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,510 +80,516 @@
     <t>Neural Architecture Search for Speech Emotion Recognition,</t>
   </si>
   <si>
+    <t>A Novel Sequential Monte Carlo Framework for Predicting Ambiguous Emotion States,</t>
+  </si>
+  <si>
+    <t>A Pre-Trained Audio-Visual Transformer for Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Representation Learning Through Cross-Modal Conditional Teacher-Student Training For Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Multi-Stage Graph Representation Learning for Dialogue-Level Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Automatic Depression Detection: an Emotional Audio-Textual Corpus and A Gru/Bilstm-Based Model,</t>
+  </si>
+  <si>
+    <t>Multi-Lingual Multi-Task Speech Emotion Recognition Using wav2vec 2.0,</t>
+  </si>
+  <si>
+    <t>SERAB: A Multi-Lingual Benchmark for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Hierarchical and Multi-View Dependency Modelling Network for Conversational Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Fusing ASR Outputs in Joint Training for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Confidence Estimation for Speech Emotion Recognition Based on the Relationship Between Emotion Categories and Primitives,</t>
+  </si>
+  <si>
+    <t>Not All Features are Equal: Selection of Robust Features for Speech Emotion Recognition in Noisy Environments,</t>
+  </si>
+  <si>
+    <t>MM-DFN: Multimodal Dynamic Fusion Network for Emotion Recognition in Conversations,</t>
+  </si>
+  <si>
+    <t>TNTC: Two-Stream Network with Transformer-Based Complementarity for Gait-Based Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Sentiment-Aware Automatic Speech Recognition Pre-Training for Enhanced Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Domain-Invariant Feature Learning for Cross Corpus Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Enhancing Privacy Through Domain Adaptive Noise Injection For Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations,</t>
+  </si>
+  <si>
+    <t>A Novel Attention-Based Gated Recurrent Unit and its Efficacy in Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks,</t>
+  </si>
+  <si>
+    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions,</t>
+  </si>
+  <si>
+    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Meta-Learning for Low-Resource Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Deep Transductive Transfer Regression Network for Cross-Corpus Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Impact of Background Noise and Contribution of Visual Information in Emotion Identification by Native Mandarin Speakers,</t>
+  </si>
+  <si>
+    <t>Language Model-Based Emotion Prediction Methods for Emotional Speech Synthesis Systems,</t>
+  </si>
+  <si>
+    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender, Emotions and Deception in a Hierarchical Framework,</t>
+  </si>
+  <si>
+    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Probing speech emotion recognition transformers for linguistic knowledge,</t>
+  </si>
+  <si>
+    <t>Cross-Speaker Emotion Transfer for Low-Resource Text-to-Speech Using Non-Parallel Voice Conversion with Pitch-Shift Data Augmentation,</t>
+  </si>
+  <si>
+    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation,</t>
+  </si>
+  <si>
+    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis,</t>
+  </si>
+  <si>
+    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning,</t>
+  </si>
+  <si>
+    <t>Text aware Emotional Text-to-speech with BERT,</t>
+  </si>
+  <si>
+    <t>Speech Emotion: Investigating Model Representations, Multi-Task Learning and Knowledge Distillation,</t>
+  </si>
+  <si>
+    <t>Automatic Detection of Expressed Emotion from Five-Minute Speech Samples: Challenges and Opportunities,</t>
+  </si>
+  <si>
+    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Context-aware Multimodal Fusion for Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation,</t>
+  </si>
+  <si>
+    <t>Extending RNN-T-based speech recognition systems with emotion and language classification,</t>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms,</t>
+  </si>
+  <si>
+    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>SpeechEQ: Speech Emotion Recognition based on Multi-scale Unified Datasets and Multitask Learning,</t>
+  </si>
+  <si>
+    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis,</t>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks,</t>
+  </si>
+  <si>
+    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning,</t>
+  </si>
+  <si>
+    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling,</t>
+  </si>
+  <si>
+    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection,</t>
+  </si>
+  <si>
+    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions,</t>
+  </si>
+  <si>
+    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier,</t>
+  </si>
+  <si>
+    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation,</t>
+  </si>
+  <si>
+    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network,</t>
+  </si>
+  <si>
+    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss,</t>
+  </si>
+  <si>
+    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition,</t>
+  </si>
+  <si>
+    <t>Temporal Context in Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Exploring emotional prototypes in a high dimensional TTS latent space,</t>
+  </si>
+  <si>
+    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit,</t>
+  </si>
+  <si>
+    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech,</t>
+  </si>
+  <si>
+    <t>Emotion Carrier Recognition from Personal Narratives,</t>
+  </si>
+  <si>
+    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia,</t>
+  </si>
+  <si>
+    <t>Emotional Prosody Control for Speech Generation,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure,</t>
+  </si>
+  <si>
+    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings,</t>
+  </si>
+  <si>
+    <t>Speaker Attentive Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability,</t>
+  </si>
+  <si>
+    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Graph Isomorphism Network for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation,</t>
+  </si>
+  <si>
+    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions,</t>
+  </si>
+  <si>
+    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Towards the Explainability of Multimodal Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech,</t>
+  </si>
+  <si>
+    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes,</t>
+  </si>
+  <si>
+    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation,</t>
+  </si>
+  <si>
+    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition,</t>
+  </si>
+  <si>
+    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition with Multi-Task Learning,</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition with Global-Aware Fusion on Multi-Scale Feature Representation,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICASSP2022</t>
+  </si>
+  <si>
+    <t>ICASSP2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memobert: Pre-Training Model with Prompt-Based Learning for Multimodal Emotion Recognition,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Selective Multi-Task Learning For Speech Emotion Recognition Using Corpora Of Different Styles,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>×</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73.90±1.31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.09% (+2.1)-72.22% (+2.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICASSP2021</t>
+  </si>
+  <si>
+    <t>模态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音-视频-文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREMA-D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音-视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP(VoxCeleb1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COGNIMUSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音-文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.87%-79.53%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECOLA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-IMPROV+CREMA-D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-IMPROV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMUMOSEI+DAIC-WOZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC (0.697-0.658)-70.22%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC (0.667 0.582 0.545)-CCC (0.757 0.627 0.671)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多数据库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1 67.88%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自建数据库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC(0.572 0.505 0.212)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MELD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion-Gait</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>步态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.97(±0.75)%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75.6%-64.9%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AuxFormer: Robust Approach to Audiovisual Emotion Recognition,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1 0.765-F1 0.717</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC(.679 0.412 0.564)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.2_81.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>56.94%_70.54%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC(78.59, 75.56)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Improv+CREMA-D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmoVox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS+EMO-DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音+视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eENTERFACE05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCC(0.6416, 0.5490, 0.1752)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.03%-56.17%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Climate and Weather: Inspecting Depression Detection via Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>A Novel Sequential Monte Carlo Framework for Predicting Ambiguous Emotion States,</t>
-  </si>
-  <si>
-    <t>A Pre-Trained Audio-Visual Transformer for Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Representation Learning Through Cross-Modal Conditional Teacher-Student Training For Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Multi-Stage Graph Representation Learning for Dialogue-Level Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Automatic Depression Detection: an Emotional Audio-Textual Corpus and A Gru/Bilstm-Based Model,</t>
-  </si>
-  <si>
-    <t>Multi-Lingual Multi-Task Speech Emotion Recognition Using wav2vec 2.0,</t>
-  </si>
-  <si>
-    <t>SERAB: A Multi-Lingual Benchmark for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Hierarchical and Multi-View Dependency Modelling Network for Conversational Emotion Recognition,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Speech Emotion Recognition Using Self-Supervised Features,</t>
-  </si>
-  <si>
-    <t>Fusing ASR Outputs in Joint Training for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Confidence Estimation for Speech Emotion Recognition Based on the Relationship Between Emotion Categories and Primitives,</t>
-  </si>
-  <si>
-    <t>Not All Features are Equal: Selection of Robust Features for Speech Emotion Recognition in Noisy Environments,</t>
-  </si>
-  <si>
-    <t>MM-DFN: Multimodal Dynamic Fusion Network for Emotion Recognition in Conversations,</t>
-  </si>
-  <si>
-    <t>TNTC: Two-Stream Network with Transformer-Based Complementarity for Gait-Based Emotion Recognition,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Multi-Modal Emotion Recognition with Self-Guided Modality Calibration,</t>
-  </si>
-  <si>
-    <t>Sentiment-Aware Automatic Speech Recognition Pre-Training for Enhanced Speech Emotion Recognition,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Speaker Normalization for Self-Supervised Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Domain-Invariant Feature Learning for Cross Corpus Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Enhancing Privacy Through Domain Adaptive Noise Injection For Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Recognition by Fusing Time Synchronous and Time Asynchronous Representations,</t>
-  </si>
-  <si>
-    <t>A Novel Attention-Based Gated Recurrent Unit and its Efficacy in Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion,</t>
-  </si>
-  <si>
-    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions,</t>
-  </si>
-  <si>
-    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Meta-Learning for Low-Resource Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Deep Transductive Transfer Regression Network for Cross-Corpus Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Impact of Background Noise and Contribution of Visual Information in Emotion Identification by Native Mandarin Speakers,</t>
-  </si>
-  <si>
-    <t>Language Model-Based Emotion Prediction Methods for Emotional Speech Synthesis Systems,</t>
-  </si>
-  <si>
-    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender, Emotions and Deception in a Hierarchical Framework,</t>
-  </si>
-  <si>
-    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Probing speech emotion recognition transformers for linguistic knowledge,</t>
-  </si>
-  <si>
-    <t>Cross-Speaker Emotion Transfer for Low-Resource Text-to-Speech Using Non-Parallel Voice Conversion with Pitch-Shift Data Augmentation,</t>
-  </si>
-  <si>
-    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation,</t>
-  </si>
-  <si>
-    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis,</t>
-  </si>
-  <si>
-    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning,</t>
-  </si>
-  <si>
-    <t>Text aware Emotional Text-to-speech with BERT,</t>
-  </si>
-  <si>
-    <t>Speech Emotion: Investigating Model Representations, Multi-Task Learning and Knowledge Distillation,</t>
-  </si>
-  <si>
-    <t>Automatic Detection of Expressed Emotion from Five-Minute Speech Samples: Challenges and Opportunities,</t>
-  </si>
-  <si>
-    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Context-aware Multimodal Fusion for Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation,</t>
-  </si>
-  <si>
-    <t>Extending RNN-T-based speech recognition systems with emotion and language classification,</t>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms,</t>
-  </si>
-  <si>
-    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>SpeechEQ: Speech Emotion Recognition based on Multi-scale Unified Datasets and Multitask Learning,</t>
-  </si>
-  <si>
-    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis,</t>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks,</t>
-  </si>
-  <si>
-    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning,</t>
-  </si>
-  <si>
-    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling,</t>
-  </si>
-  <si>
-    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection,</t>
-  </si>
-  <si>
-    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions,</t>
-  </si>
-  <si>
-    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier,</t>
-  </si>
-  <si>
-    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation,</t>
-  </si>
-  <si>
-    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network,</t>
-  </si>
-  <si>
-    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss,</t>
-  </si>
-  <si>
-    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition,</t>
-  </si>
-  <si>
-    <t>Temporal Context in Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Exploring emotional prototypes in a high dimensional TTS latent space,</t>
-  </si>
-  <si>
-    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit,</t>
-  </si>
-  <si>
-    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech,</t>
-  </si>
-  <si>
-    <t>Emotion Carrier Recognition from Personal Narratives,</t>
-  </si>
-  <si>
-    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia,</t>
-  </si>
-  <si>
-    <t>Emotional Prosody Control for Speech Generation,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure,</t>
-  </si>
-  <si>
-    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings,</t>
-  </si>
-  <si>
-    <t>Speaker Attentive Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability,</t>
-  </si>
-  <si>
-    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Graph Isomorphism Network for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation,</t>
-  </si>
-  <si>
-    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions,</t>
-  </si>
-  <si>
-    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Towards the Explainability of Multimodal Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech,</t>
-  </si>
-  <si>
-    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes,</t>
-  </si>
-  <si>
-    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation,</t>
-  </si>
-  <si>
-    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition,</t>
-  </si>
-  <si>
-    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition with Multi-Task Learning,</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition with Global-Aware Fusion on Multi-Scale Feature Representation,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICASSP2022</t>
-  </si>
-  <si>
-    <t>ICASSP2022</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>√</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memobert: Pre-Training Model with Prompt-Based Learning for Multimodal Emotion Recognition,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Selective Multi-Task Learning For Speech Emotion Recognition Using Corpora Of Different Styles,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>×</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73.90±1.31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.09% (+2.1)-72.22% (+2.5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICASSP2021</t>
-  </si>
-  <si>
-    <t>模态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音-视频-文本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREMA-D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音-视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP(VoxCeleb1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COGNIMUSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音-文本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.87%-79.53%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECOLA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-IMPROV+CREMA-D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-IMPROV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMUMOSEI+DAIC-WOZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC (0.697-0.658)-70.22%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC (0.667 0.582 0.545)-CCC (0.757 0.627 0.671)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多数据库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F1 67.88%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自建数据库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC(0.572 0.505 0.212)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion-Gait</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>步态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>85.97(±0.75)%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75.6%-64.9%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AuxFormer: Robust Approach to Audiovisual Emotion Recognition,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F1 0.765-F1 0.717</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC(.679 0.412 0.564)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74.2_81.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>56.94%_70.54%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC(78.59, 75.56)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Improv+CREMA-D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EmoVox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS+EMO-DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音+视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eENTERFACE05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCC(0.6416, 0.5490, 0.1752)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.03%-56.17%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -911,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -943,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -951,59 +967,59 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G4" s="3">
         <v>0.62680000000000002</v>
@@ -1014,13 +1030,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G5" s="4">
         <v>0.76</v>
@@ -1031,13 +1047,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G6" s="3">
         <v>0.68189999999999995</v>
@@ -1048,13 +1064,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G7" s="3">
         <v>0.53510000000000002</v>
@@ -1065,95 +1081,95 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>159</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G13" s="3">
         <v>0.6976</v>
@@ -1161,16 +1177,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G14" s="3">
         <v>0.64100000000000001</v>
@@ -1178,16 +1194,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G15" s="3">
         <v>0.64100000000000001</v>
@@ -1195,16 +1211,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G16" s="3">
         <v>0.65100000000000002</v>
@@ -1212,33 +1228,33 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>160</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G18" s="3">
         <v>0.77759999999999996</v>
@@ -1246,16 +1262,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G19" s="3">
         <v>0.63400000000000001</v>
@@ -1263,16 +1279,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G20" s="3">
         <v>0.36580000000000001</v>
@@ -1280,33 +1296,33 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G22" s="3">
         <v>0.68210000000000004</v>
@@ -1314,115 +1330,115 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>161</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>162</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G29" s="3">
         <v>0.57599999999999996</v>
@@ -1430,16 +1446,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G30" s="3">
         <v>0.52090000000000003</v>
@@ -1447,16 +1463,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G31" s="3">
         <v>0.77359999999999995</v>
@@ -1464,16 +1480,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G32" s="3">
         <v>0.66900000000000004</v>
@@ -1481,30 +1497,30 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G34" s="3">
         <v>0.7046</v>
@@ -1512,16 +1528,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G35" s="3">
         <v>0.80830000000000002</v>
@@ -1529,33 +1545,33 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G37" s="3">
         <v>0.60429999999999995</v>
@@ -1563,412 +1579,412 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2022-11-17 14:52:41
</commit_message>
<xml_diff>
--- a/情感识别论文统计.xlsx
+++ b/情感识别论文统计.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA277412-2972-43CD-B248-C12330EEB26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAA68B2-A74F-4409-875A-4F7AD9D00A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$113</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -597,7 +599,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +611,14 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -630,10 +640,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -645,9 +658,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="警告文本" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -925,10 +940,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1041,7 @@
         <v>0.62680000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1075,7 @@
         <v>0.68189999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1126,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1124,7 +1140,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1175,7 +1191,7 @@
         <v>0.6976</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1294,7 +1310,7 @@
         <v>0.36580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1344,7 @@
         <v>0.68210000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1362,7 +1378,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>145</v>
       </c>
@@ -1386,7 +1402,7 @@
       <c r="B26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1495,7 +1511,7 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1526,7 +1542,7 @@
         <v>0.7046</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>164</v>
       </c>
@@ -1543,7 +1559,7 @@
         <v>0.80830000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1622,372 +1638,387 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G113" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="IEMOCAP"/>
+        <filter val="IEMOCAP(VoxCeleb1)"/>
+        <filter val="IEMOCAP+CMUMOSEI+DAIC-WOZ"/>
+        <filter val="IEMOCAP+MELD"/>
+        <filter val="IEMOCAP+MSP-IMPROV"/>
+        <filter val="IEMOCAP+MSP-Improv+CREMA-D"/>
+        <filter val="IEMOCAP+MSP-Podcast"/>
+        <filter val="IEMOCAP+RAVDESS+EMO-DB"/>
+        <filter val="多数据库"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2022-11-26 21:28:28
</commit_message>
<xml_diff>
--- a/情感识别论文统计.xlsx
+++ b/情感识别论文统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF43D84C-6FC4-4609-B52C-5DA0964B73A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22407AC3-D20F-4A51-82F5-10B70B438975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1104" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -455,337 +455,341 @@
     <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
   </si>
   <si>
+    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
+  </si>
+  <si>
+    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
+  </si>
+  <si>
+    <t>Temporal Context in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
+  </si>
+  <si>
+    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
+  </si>
+  <si>
+    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
+  </si>
+  <si>
+    <t>Emotion Carrier Recognition from Personal Narratives</t>
+  </si>
+  <si>
+    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
+  </si>
+  <si>
+    <t>Emotional Prosody Control for Speech Generation</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
+  </si>
+  <si>
+    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
+  </si>
+  <si>
+    <t>Speaker Attentive Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
+  </si>
+  <si>
+    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
+  </si>
+  <si>
+    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
+  </si>
+  <si>
+    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
+  </si>
+  <si>
+    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
+  </si>
+  <si>
+    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
+  </si>
+  <si>
+    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMU-MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音+视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+ESD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmoDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.5±1.0%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wF1 78.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSI+CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音-视频-文本 </t>
+  </si>
+  <si>
+    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本 </t>
+  </si>
+  <si>
+    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wf1 65.85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MELD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emo-DB+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.6± 4.7% - 61.7±9.2%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMUMOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+NNIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-IMPROV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.613 ± 0.018%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+Att-HACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS+Emo-DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音 </t>
+  </si>
+  <si>
+    <t>67.2 ± 0.7%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.90 ± 4.31%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本   </t>
+  </si>
+  <si>
     <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
-  </si>
-  <si>
-    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
-  </si>
-  <si>
-    <t>Temporal Context in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
-  </si>
-  <si>
-    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
-  </si>
-  <si>
-    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
-  </si>
-  <si>
-    <t>Emotion Carrier Recognition from Personal Narratives</t>
-  </si>
-  <si>
-    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
-  </si>
-  <si>
-    <t>Emotional Prosody Control for Speech Generation</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
-  </si>
-  <si>
-    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
-  </si>
-  <si>
-    <t>Speaker Attentive Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
-  </si>
-  <si>
-    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
-  </si>
-  <si>
-    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
-  </si>
-  <si>
-    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
-  </si>
-  <si>
-    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
-  </si>
-  <si>
-    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Speech Emotion Recognition with Multi-Task Learning</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMU-MOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音+视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+ESD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EmoDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>87.5±1.0%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wF1 78.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSI+CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音-视频-文本 </t>
-  </si>
-  <si>
-    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本 </t>
-  </si>
-  <si>
-    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wf1 65.85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emo-DB+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.6± 4.7% - 61.7±9.2%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMUMOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+NNIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-IMPROV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.613 ± 0.018%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+Att-HACK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS+Emo-DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音 </t>
-  </si>
-  <si>
-    <t>67.2 ± 0.7%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95.90 ± 4.31%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1148,10 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1278,7 @@
         <v>84.45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
@@ -1321,7 +1326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>79.52</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -1403,7 +1408,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>77.36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -1497,7 +1502,7 @@
         <v>77.099999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -1518,7 +1523,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
@@ -1542,7 +1547,7 @@
         <v>76.31</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>75.930000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -1678,7 +1683,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -1724,7 +1729,7 @@
         <v>73.22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
@@ -1790,7 +1795,7 @@
         <v>72.48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>70.540000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -1903,7 +1908,7 @@
         <v>70.11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -1944,7 +1949,7 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
@@ -1965,7 +1970,7 @@
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>94</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>67.42</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
@@ -2049,7 +2054,7 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>65.53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -2119,13 +2124,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>53</v>
@@ -2143,7 +2148,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>55</v>
@@ -2152,7 +2157,7 @@
         <v>54</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G44" s="2">
         <v>73.22</v>
@@ -2166,13 +2171,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>59</v>
@@ -2187,21 +2192,21 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J46" s="10">
         <v>63.4</v>
@@ -2210,15 +2215,15 @@
         <v>60.43</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>59</v>
@@ -2230,15 +2235,15 @@
         <v>58.19</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J48" s="10">
         <v>68.900000000000006</v>
@@ -2247,21 +2252,21 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H49" s="1"/>
       <c r="J49" s="10">
@@ -2273,7 +2278,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>55</v>
@@ -2295,18 +2300,18 @@
         <v>0.77029999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2317,15 +2322,15 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>53</v>
@@ -2336,15 +2341,15 @@
         <v>0.68189999999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2355,15 +2360,15 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2376,7 +2381,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>55</v>
@@ -2398,9 +2403,9 @@
         <v>0.62680000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>55</v>
@@ -2416,7 +2421,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>55</v>
@@ -2425,7 +2430,7 @@
         <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G57" s="6">
         <v>0.84450000000000003</v>
@@ -2440,16 +2445,16 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H58" s="1"/>
       <c r="J58" s="10">
@@ -2461,13 +2466,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>59</v>
@@ -2485,7 +2490,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>55</v>
@@ -2507,21 +2512,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H61" s="1"/>
       <c r="J61" s="10">
@@ -2531,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>100</v>
       </c>
@@ -2549,7 +2554,7 @@
     </row>
     <row r="63" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>55</v>
@@ -2591,7 +2596,7 @@
     </row>
     <row r="65" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>55</v>
@@ -2610,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>102</v>
       </c>
@@ -2628,7 +2633,7 @@
     </row>
     <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>55</v>
@@ -2637,7 +2642,7 @@
         <v>54</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G67" s="8">
         <v>0.73040000000000005</v>
@@ -2652,13 +2657,13 @@
     </row>
     <row r="68" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G68" s="8">
         <v>0.63400000000000001</v>
@@ -2677,7 +2682,7 @@
         <v>55</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G69" s="8">
         <v>0.68169999999999997</v>
@@ -2698,7 +2703,7 @@
         <v>55</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G70" s="8">
         <v>0.68899999999999995</v>
@@ -2709,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>105</v>
       </c>
@@ -2722,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>106</v>
       </c>
@@ -2734,13 +2739,13 @@
     </row>
     <row r="73" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G73" s="8">
         <v>0.80030000000000001</v>
@@ -2750,13 +2755,13 @@
     </row>
     <row r="74" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G74" s="8">
         <v>0.76100000000000001</v>
@@ -2764,9 +2769,9 @@
       <c r="H74" s="8"/>
       <c r="J74" s="11"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>55</v>
@@ -2776,13 +2781,13 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G76" s="6">
         <v>0.70399999999999996</v>
@@ -2791,19 +2796,19 @@
     </row>
     <row r="77" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J77" s="11"/>
     </row>
     <row r="78" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>56</v>
@@ -2812,25 +2817,25 @@
         <v>54</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J78" s="11"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G79" s="6">
         <v>0.66900000000000004</v>
@@ -2839,169 +2844,169 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G80" s="6">
         <v>0.77100000000000002</v>
       </c>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G88" s="6">
         <v>0.76100000000000001</v>
       </c>
       <c r="H88" s="6"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="B92" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>54</v>
@@ -3013,10 +3018,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>54</v>
@@ -3028,10 +3033,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>54</v>
@@ -3043,63 +3048,63 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G96" s="6">
         <v>0.61399999999999999</v>
       </c>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G98" s="6">
         <v>0.73499999999999999</v>
       </c>
       <c r="H98" s="6"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G100" s="6">
         <v>0.6169</v>
@@ -3108,16 +3113,16 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G101" s="6">
         <v>0.75</v>
@@ -3126,35 +3131,35 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G102" s="6">
         <v>0.65600000000000003</v>
       </c>
       <c r="H102" s="6"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>54</v>
@@ -3166,10 +3171,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>54</v>
@@ -3177,22 +3182,22 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>54</v>
@@ -3203,7 +3208,29 @@
       <c r="H107" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="IEMOCAP"/>
+        <filter val="IEMOCAP(VoxCeleb1)"/>
+        <filter val="IEMOCAP+Att-HACK"/>
+        <filter val="IEMOCAP+CMUMOSEI+DAIC-WOZ"/>
+        <filter val="IEMOCAP+CMUMOSI"/>
+        <filter val="IEMOCAP+CMU-MOSI"/>
+        <filter val="IEMOCAP+CREMA-D+MSP-Improv"/>
+        <filter val="IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast"/>
+        <filter val="IEMOCAP+DailyDialog+MELD+EmoryNLP"/>
+        <filter val="IEMOCAP+ESD"/>
+        <filter val="IEMOCAP+MELD"/>
+        <filter val="IEMOCAP+MSP-IMPROV"/>
+        <filter val="IEMOCAP+MSP-Improv+CREMA-D"/>
+        <filter val="IEMOCAP+MSP-Podcast"/>
+        <filter val="IEMOCAP+NNIME"/>
+        <filter val="IEMOCAP+RAVDESS"/>
+        <filter val="IEMOCAP+RAVDESS+EMO-DB"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2022-12-06 23:25:49
</commit_message>
<xml_diff>
--- a/情感识别论文统计.xlsx
+++ b/情感识别论文统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22407AC3-D20F-4A51-82F5-10B70B438975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4178431A-BBBF-4781-8649-70D7D7AAB16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1104" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5448" yWindow="8820" windowWidth="15276" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="201">
   <si>
     <t>论文</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -398,397 +398,403 @@
     <t>Enhancing Privacy Through Domain Adaptive Noise Injection For Speech Emotion Recognition</t>
   </si>
   <si>
+    <t>Emotion Recognition by Fusing Time Synchronous and Time Asynchronous Representations</t>
+  </si>
+  <si>
+    <t>A Novel Attention-Based Gated Recurrent Unit and its Efficacy in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks</t>
+  </si>
+  <si>
+    <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion</t>
+  </si>
+  <si>
+    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
+  </si>
+  <si>
+    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
+  </si>
+  <si>
+    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
+  </si>
+  <si>
+    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
+  </si>
+  <si>
+    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
+  </si>
+  <si>
+    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
+  </si>
+  <si>
+    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
+  </si>
+  <si>
+    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
+  </si>
+  <si>
+    <t>Temporal Context in Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
+  </si>
+  <si>
+    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
+  </si>
+  <si>
+    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
+  </si>
+  <si>
+    <t>Emotion Carrier Recognition from Personal Narratives</t>
+  </si>
+  <si>
+    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
+  </si>
+  <si>
+    <t>Emotional Prosody Control for Speech Generation</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
+  </si>
+  <si>
+    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
+  </si>
+  <si>
+    <t>Speaker Attentive Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
+  </si>
+  <si>
+    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
+  </si>
+  <si>
+    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
+  </si>
+  <si>
+    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
+  </si>
+  <si>
+    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
+  </si>
+  <si>
+    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
+  </si>
+  <si>
+    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
+  </si>
+  <si>
+    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+  </si>
+  <si>
+    <t>Interspeech2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMU-MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音+视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+ESD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmoDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.5±1.0%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wF1 78.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-MOSI+CMU-MOSEI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音-视频-文本 </t>
+  </si>
+  <si>
+    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本 </t>
+  </si>
+  <si>
+    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wf1 65.85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MELD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emo-DB+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.6± 4.7% - 61.7±9.2%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-Improv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CMUMOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+NNIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+MSP-IMPROV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.613 ± 0.018%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+Att-HACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IEMOCAP+RAVDESS+Emo-DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音 </t>
+  </si>
+  <si>
+    <t>67.2 ± 0.7%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.90 ± 4.31%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">语音+文本   </t>
+  </si>
+  <si>
+    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech Emotion Recognition with Multi-Task Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Towards Transferable Speech Emotion Representation: On Loss Functions for Cross-Lingual Latent Representations</t>
-  </si>
-  <si>
-    <t>Emotion Recognition by Fusing Time Synchronous and Time Asynchronous Representations</t>
-  </si>
-  <si>
-    <t>A Novel Attention-Based Gated Recurrent Unit and its Efficacy in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Disentanglement for Audio-Visual Emotion Recognition Using Multitask Setup</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Using Quaternion Convolutional Neural Networks</t>
-  </si>
-  <si>
-    <t>Multimodal Emotion Recognition with Capsule Graph Convolutional Based Representation Fusion</t>
-  </si>
-  <si>
-    <t>Deepemocluster: a Semi-Supervised Framework for Latent Cluster Representation of Speech Emotions</t>
-  </si>
-  <si>
-    <t>Representation Learning with Spectro-Temporal-Channel Attention for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Domain-Adversarial Autoencoder with Attention Based Feature Level Fusion for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>MAEC: Multi-Instance Learning with an Adversarial Auto-Encoder-Based Classifier for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Meta-Learning for Low-Resource Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multi-level Fusion of Wav2vec 2.0 and BERT for Multimodal Emotion Recognition</t>
-  </si>
-  <si>
-    <t>ADFF: Attention Based Deep Feature Fusion Approach for Music Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Multiple Enhancements to LSTM for Learning Emotion-Salient Features in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Using Self-Supervised Learning with Domain-Specific Audiovisual Tasks</t>
-  </si>
-  <si>
-    <t>Semi-FedSER: Semi-supervised Learning for Speech Emotion Recognition On Federated Learning using Multiview Pseudo-Labeling</t>
-  </si>
-  <si>
-    <t>Positional Encoding for Capturing Modality Specific Cadence for Emotion Detection</t>
-  </si>
-  <si>
-    <t>Telling self-defining memories: An acoustic study of natural emotional speech productions</t>
-  </si>
-  <si>
-    <t>Exploiting Co-occurrence Frequency of Emotions in Perceptual Evaluations To Train A Speech Emotion Classifier</t>
-  </si>
-  <si>
-    <t>Speaker Trait Enhancement for Cochlear Implant Users: A Case Study for Speaker Emotion Perception</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Generation using an Attention-based Variational Recurrent Neural Network</t>
-  </si>
-  <si>
-    <t>Multi-Corpus Speech Emotion Recognition for Unseen Corpus Using Corpus-Wise Weights in Classification Loss</t>
-  </si>
-  <si>
-    <t>Temporal Context in Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Mutual Correlation in Multimodal Transformer for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Exploring emotional prototypes in a high dimensional TTS latent space</t>
-  </si>
-  <si>
-    <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
-  </si>
-  <si>
-    <t>Acoustic and Prosodic Correlates of Emotions in Urdu Speech</t>
-  </si>
-  <si>
-    <t>Emotion Carrier Recognition from Personal Narratives</t>
-  </si>
-  <si>
-    <t>Stochastic Process Regression for Cross-Cultural Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Audio-Visual Recognition of Emotional Engagement of People with Dementia</t>
-  </si>
-  <si>
-    <t>Emotional Prosody Control for Speech Generation</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition Based on Attention Weight Correction Using Word-Level Confidence Measure</t>
-  </si>
-  <si>
-    <t>Annotation Confidence vs. Training Sample Size: Trade-Off Solution for Partially-Continuous Categorical Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Emotion Recognition from Speech Using wav2vec 2.0 Embeddings</t>
-  </si>
-  <si>
-    <t>Speaker Attentive Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Emotional Text-to-Speech Synthesis with Improved Emotion Discriminability</t>
-  </si>
-  <si>
-    <t>Graph Isomorphism Network for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition via Multi-Level Cross-Modal Distillation</t>
-  </si>
-  <si>
-    <t>Acted vs. Improvised: Domain Adaptation for Elicitation Approaches in Audio-Visual Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Learning Fine-Grained Cross Modality Excitement for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Separation of Emotional and Reconstruction Embeddings on Ladder Network to Improve Speech Emotion Recognition Robustness in Noisy Conditions</t>
-  </si>
-  <si>
-    <t>Applying TDNN Architectures for Analyzing Duration Dependencies on Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Towards the Explainability of Multimodal Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>Acoustic Features and Neural Representations for Categorical Emotion Recognition from Speech</t>
-  </si>
-  <si>
-    <t>Audio-Visual Speech Emotion Recognition by Disentangling Emotion and Identity Attributes</t>
-  </si>
-  <si>
-    <t>An Improved StarGAN for Emotional Voice Conversion: Enhancing Voice Quality and Data Augmentation</t>
-  </si>
-  <si>
-    <t>Metric Learning Based Feature Representation with Gated Fusion Model for Speech Emotion Recognition</t>
-  </si>
-  <si>
-    <t>EMOVIE: A Mandarin Emotion Speech Dataset with a Simple Emotional Text-to-Speech Model</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-  </si>
-  <si>
-    <t>Interspeech2021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exploiting Fine-tuning of Self-supervised Learning Models for Improving Bi-modal Sentiment Analysis and Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMU-MOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Audio-Visual Domain Adaptation Feature Fusion for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音+视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generative Data Augmentation Guided by Triplet Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+ESD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complex Paralinguistic Analysis of Speech: Predicting Gender Emotions and Deception in a Hierarchical Framework</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EmoDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>87.5±1.0%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Analysis of Self-Supervised Learning and Dimensionality Reduction Methods in Clustering-Based Active Learning for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMO-DB+eNTERFACE+FESC+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Probing speech emotion recognition transformers for linguistic knowledge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interactive Co-Learning with Cross-Modal Transformer for Audio-Visual Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wF1 78.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Performance Improvement of Speech Emotion Recognition by Neutral Speech Detection Using Autoencoder and Intermediate Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word-wise Sparse Attention for Multimodal Sentiment Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMU-MOSI+CMU-MOSEI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音-视频-文本 </t>
-  </si>
-  <si>
-    <t>Mind the gap: On the value of silence representations to lexical-based speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition in the Wild using Multi-task and Adversarial Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion: Investigating Model Representations Multi-Task Learning and Knowledge Distillation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Feature Representation Based on Cascaded Attention Network with Adversarial Joint Loss for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coupled Discriminant Subspace Alignment for Cross-database Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Context-aware Multimodal Fusion for Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本 </t>
-  </si>
-  <si>
-    <t>The Emotion is Not One-hot Encoding: Learning with Grayscale Label for Emotion Recognition in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+DailyDialog+MELD+EmoryNLP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wf1 65.85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extending RNN-T-based speech recognition systems with emotion and language classification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Improving Speech Emotion Recognition Through Focus and Calibration Attention Mechanisms</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discriminative Adversarial Learning for Speaker Independent Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emo-DB+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.6± 4.7% - 61.7±9.2%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User-Level Differential Privacy against Attribute Inference Attack of Speech Emotion Recognition on Federated Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-Improv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CMUMOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+NNIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+MSP-IMPROV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Graph Isomorphism Network with Weighted Multiple Aggregators for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Magnitude and Phase based Speech Representation Learning using Autoencoder for Classifying Speech Emotions using Deep Canonical Correlation Analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interpretabilty of Speech Emotion Recognition modelled using Self-Supervised Speech and Text Pre-Trained Embeddings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recurrent multi-head attention fusion network for combining audio and text for speech emotion recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion-Shift Aware CRF for Decoding Emotion Sequence in Conversation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.613 ± 0.018%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+Att-HACK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEMOCAP+RAVDESS+Emo-DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音 </t>
-  </si>
-  <si>
-    <t>67.2 ± 0.7%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95.90 ± 4.31%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">语音+文本   </t>
-  </si>
-  <si>
-    <t>CTA-RNN: Channel and Temporal-wise Attention RNN leveraging Pre-trained ASR Embeddings for Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time-Frequency Representation Learning with Graph Convolutional Network for Dialogue-Level Speech Emotion Recognition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Speech Emotion Recognition Framework for Better Discrimination of Confusions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech Emotion Recognition with Multi-Task Learning</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1155,15 +1161,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="43.77734375" style="2" customWidth="1"/>
@@ -1198,24 +1204,21 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8">
+        <v>0.7248</v>
       </c>
       <c r="J2" s="10">
         <v>75.099999999999994</v>
@@ -1225,7 +1228,7 @@
         <v>100.21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -1251,24 +1254,21 @@
         <v>84.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="3">
-        <v>0.62680000000000002</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="H4" s="3"/>
       <c r="J4" s="10">
@@ -1280,19 +1280,16 @@
     </row>
     <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.76</v>
+        <v>16</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="10">
@@ -1302,21 +1299,21 @@
         <v>83.19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.68189999999999995</v>
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="H6" s="3"/>
       <c r="J6" s="10">
@@ -1327,20 +1324,17 @@
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>65</v>
+      <c r="A7" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.53510000000000002</v>
+        <v>134</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.79520000000000002</v>
       </c>
       <c r="H7" s="3"/>
       <c r="J7" s="10">
@@ -1350,27 +1344,19 @@
         <v>80.03</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="L8" s="1">
         <v>79.53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1392,17 +1378,17 @@
       </c>
     </row>
     <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>68</v>
+      <c r="A10" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>134</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.65600000000000003</v>
       </c>
       <c r="L10" s="1">
         <v>78.5</v>
@@ -1410,20 +1396,12 @@
     </row>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="J11" s="10">
         <v>69.760000000000005</v>
       </c>
@@ -1431,7 +1409,7 @@
         <v>78.150000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1454,22 +1432,14 @@
         <v>77.760000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.6976</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="3"/>
       <c r="J13" s="10">
         <v>63.4</v>
@@ -1504,19 +1474,19 @@
     </row>
     <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="3">
-        <v>0.64100000000000001</v>
+        <v>0.53510000000000002</v>
       </c>
       <c r="H15" s="3"/>
       <c r="L15" s="1">
@@ -1524,20 +1494,17 @@
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>74</v>
+      <c r="A16" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.65100000000000002</v>
+        <v>134</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.70819999999999994</v>
       </c>
       <c r="H16" s="3"/>
       <c r="J16" s="10">
@@ -1549,19 +1516,16 @@
     </row>
     <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="J17" s="10">
         <v>0.75600000000000001</v>
@@ -1570,7 +1534,7 @@
         <v>76.17</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -1591,42 +1555,31 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.63400000000000001</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="3"/>
       <c r="L19" s="1">
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>78</v>
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.36580000000000001</v>
+        <v>134</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.6169</v>
       </c>
       <c r="H20" s="3"/>
       <c r="J20" s="10">
@@ -1636,21 +1589,24 @@
         <v>75.930000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>35</v>
+        <v>139</v>
+      </c>
+      <c r="G21" s="2">
+        <v>73.22</v>
       </c>
       <c r="J21" s="10">
         <v>57.6</v>
@@ -1659,7 +1615,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -1706,7 +1662,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -1731,25 +1687,17 @@
     </row>
     <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G25" s="1"/>
       <c r="L25" s="1">
         <v>73.040000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -1772,22 +1720,14 @@
         <v>72.83</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G27" s="1"/>
       <c r="J27" s="10">
         <v>0.77029999999999998</v>
       </c>
@@ -1797,17 +1737,12 @@
     </row>
     <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G28" s="1"/>
       <c r="J28" s="10">
         <v>76.31</v>
       </c>
@@ -1815,21 +1750,21 @@
         <v>70.819999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.57599999999999996</v>
+        <v>19</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="H29" s="3"/>
       <c r="J29" s="10">
@@ -1841,19 +1776,19 @@
     </row>
     <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>32</v>
+        <v>143</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.52090000000000003</v>
+        <v>59</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="H30" s="3"/>
       <c r="J30" s="10">
@@ -1863,21 +1798,21 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="3">
-        <v>0.77359999999999995</v>
+        <v>0.36580000000000001</v>
       </c>
       <c r="H31" s="3"/>
       <c r="J31" s="10">
@@ -1887,39 +1822,34 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.66900000000000004</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G32" s="1"/>
       <c r="H32" s="3"/>
       <c r="L32" s="1">
         <v>70.11</v>
       </c>
     </row>
     <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>19</v>
+      <c r="A33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8">
+        <v>0.76100000000000001</v>
       </c>
       <c r="J33" s="10">
         <v>84.5</v>
@@ -1928,21 +1858,21 @@
         <v>69.760000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="G34" s="3">
-        <v>0.7046</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="H34" s="3"/>
       <c r="L34" s="1">
@@ -1957,13 +1887,13 @@
         <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.80830000000000002</v>
+        <v>16</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H35" s="3"/>
       <c r="L35" s="1">
@@ -1972,39 +1902,39 @@
     </row>
     <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>169</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="L36" s="1">
         <v>68.17</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0.60429999999999995</v>
+        <v>59</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.76170000000000004</v>
       </c>
       <c r="H37" s="3"/>
       <c r="J37" s="10">
@@ -2016,16 +1946,16 @@
     </row>
     <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J38" s="10">
         <v>84.45</v>
@@ -2034,38 +1964,35 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="L39" s="1">
         <v>66.900000000000006</v>
       </c>
     </row>
     <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>16</v>
+      <c r="G40" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="J40" s="10">
         <v>76.5</v>
@@ -2074,9 +2001,9 @@
         <v>65.599999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>56</v>
@@ -2100,20 +2027,12 @@
     </row>
     <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42" s="3">
-        <v>0.41099999999999998</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G42" s="1"/>
       <c r="H42" s="3"/>
       <c r="J42" s="10">
         <v>72.48</v>
@@ -2122,15 +2041,15 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>53</v>
@@ -2146,21 +2065,21 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="2">
-        <v>73.22</v>
+        <v>16</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.77359999999999995</v>
       </c>
       <c r="J44" s="10">
         <v>67.42</v>
@@ -2169,21 +2088,21 @@
         <v>61.69</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>142</v>
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G45" s="2">
-        <v>58.19</v>
+      <c r="G45" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="J45" s="10">
         <v>73.040000000000006</v>
@@ -2194,20 +2113,12 @@
     </row>
     <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>146</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G46" s="1"/>
       <c r="J46" s="10">
         <v>63.4</v>
       </c>
@@ -2216,17 +2127,20 @@
       </c>
     </row>
     <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>59</v>
+      <c r="A47" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8">
+        <v>0.80030000000000001</v>
       </c>
       <c r="J47" s="10">
         <v>68.17</v>
@@ -2237,14 +2151,12 @@
     </row>
     <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G48" s="1"/>
       <c r="J48" s="10">
         <v>68.900000000000006</v>
       </c>
@@ -2254,19 +2166,19 @@
     </row>
     <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>153</v>
+        <v>16</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.57599999999999996</v>
       </c>
       <c r="H49" s="1"/>
       <c r="J49" s="10">
@@ -2276,9 +2188,9 @@
         <v>36.58</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>55</v>
@@ -2302,16 +2214,16 @@
     </row>
     <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2324,13 +2236,13 @@
     </row>
     <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>53</v>
@@ -2343,13 +2255,10 @@
     </row>
     <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2362,13 +2271,10 @@
     </row>
     <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2379,21 +2285,21 @@
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G55" s="6">
-        <v>0.76170000000000004</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="H55" s="6"/>
       <c r="J55" s="10">
@@ -2405,12 +2311,20 @@
     </row>
     <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>64</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G56" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0.68189999999999995</v>
+      </c>
       <c r="H56" s="1"/>
       <c r="J56" s="10">
         <v>76.099999999999994</v>
@@ -2419,9 +2333,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>55</v>
@@ -2430,7 +2344,7 @@
         <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G57" s="6">
         <v>0.84450000000000003</v>
@@ -2443,18 +2357,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>167</v>
+        <v>6</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0.63400000000000001</v>
       </c>
       <c r="H58" s="1"/>
       <c r="J58" s="10">
@@ -2464,21 +2381,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G59" s="6">
-        <v>0.76500000000000001</v>
+      <c r="G59" s="2">
+        <v>58.19</v>
       </c>
       <c r="H59" s="6"/>
       <c r="J59" s="10">
@@ -2488,21 +2405,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>170</v>
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="G60" s="6">
-        <v>0.72829999999999995</v>
+        <v>0.65529999999999999</v>
       </c>
       <c r="H60" s="6"/>
       <c r="J60" s="10">
@@ -2514,19 +2428,19 @@
     </row>
     <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>171</v>
+        <v>75</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>173</v>
+        <v>16</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="H61" s="1"/>
       <c r="J61" s="10">
@@ -2538,12 +2452,20 @@
     </row>
     <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.72829999999999995</v>
+      </c>
       <c r="H62" s="1"/>
       <c r="J62" s="10">
         <v>61.4</v>
@@ -2552,19 +2474,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G63" s="8">
-        <v>0.7248</v>
-      </c>
+    <row r="63" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
       <c r="H63" s="8"/>
       <c r="J63" s="11">
         <v>73.5</v>
@@ -2573,18 +2494,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G64" s="8">
-        <v>0.70109999999999995</v>
+    <row r="64" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="H64" s="8"/>
       <c r="J64" s="11">
@@ -2594,18 +2520,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>55</v>
+    <row r="65" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G65" s="8">
-        <v>0.67420000000000002</v>
+        <v>178</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="6">
+        <v>0.73499999999999999</v>
       </c>
       <c r="H65" s="8"/>
       <c r="J65" s="11">
@@ -2617,12 +2546,20 @@
     </row>
     <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G66" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="H66" s="1"/>
       <c r="J66" s="10">
         <v>65.599999999999994</v>
@@ -2631,9 +2568,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>55</v>
@@ -2642,7 +2579,7 @@
         <v>54</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G67" s="8">
         <v>0.73040000000000005</v>
@@ -2655,38 +2592,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G68" s="8">
-        <v>0.63400000000000001</v>
-      </c>
+    <row r="68" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="2"/>
       <c r="H68" s="8"/>
       <c r="J68" s="11"/>
       <c r="L68" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>55</v>
+    <row r="69" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G69" s="8">
-        <v>0.68169999999999997</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
       <c r="H69" s="8"/>
       <c r="J69" s="11">
         <v>78.150000000000006</v>
@@ -2695,18 +2636,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G70" s="8">
-        <v>0.68899999999999995</v>
+        <v>179</v>
       </c>
       <c r="H70" s="8"/>
       <c r="J70" s="11"/>
@@ -2716,12 +2654,20 @@
     </row>
     <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G71" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="3">
+        <v>0.64100000000000001</v>
+      </c>
       <c r="H71" s="1"/>
       <c r="L71" s="1">
         <v>0</v>
@@ -2729,86 +2675,118 @@
     </row>
     <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G72" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G72" s="3">
+        <v>0.80830000000000002</v>
+      </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="G73" s="8">
-        <v>0.80030000000000001</v>
+    <row r="73" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="4">
+        <v>0.76</v>
       </c>
       <c r="H73" s="8"/>
       <c r="J73" s="11"/>
     </row>
-    <row r="74" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>196</v>
+        <v>100</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="G74" s="8">
-        <v>0.76100000000000001</v>
+        <v>0.70109999999999995</v>
       </c>
       <c r="H74" s="8"/>
       <c r="J74" s="11"/>
     </row>
     <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G75" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="3">
+        <v>0.6976</v>
+      </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>108</v>
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G76" s="6">
-        <v>0.70399999999999996</v>
+        <v>6</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>181</v>
+    <row r="77" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="J77" s="11"/>
     </row>
-    <row r="78" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>56</v>
@@ -2817,43 +2795,43 @@
         <v>54</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J78" s="11"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>137</v>
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G79" s="6">
-        <v>0.66900000000000004</v>
+        <v>175</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="8">
+        <v>0.68899999999999995</v>
       </c>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G80" s="6">
         <v>0.77100000000000002</v>
@@ -2862,86 +2840,122 @@
     </row>
     <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G81" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G83" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" s="3">
+        <v>0.60429999999999995</v>
+      </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G84" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" s="3">
+        <v>0.62680000000000002</v>
+      </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G85" s="1"/>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="8">
+        <v>0.68169999999999997</v>
+      </c>
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G87" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" s="3">
+        <v>0.65100000000000002</v>
+      </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G88" s="6">
         <v>0.76100000000000001</v>
@@ -2949,287 +2963,323 @@
       <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G89" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
-        <v>121</v>
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>180</v>
+        <v>8</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>193</v>
+        <v>16</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
-        <v>122</v>
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="3">
+        <v>0.7046</v>
+      </c>
+      <c r="H93" s="6"/>
+    </row>
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G94" s="6">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="H94" s="6"/>
+    </row>
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G95" s="6">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H95" s="6"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96" s="6"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C93" s="7" t="s">
+      <c r="B97" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C97" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G93" s="6">
-        <v>0.75929999999999997</v>
-      </c>
-      <c r="H93" s="6"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G94" s="6">
-        <v>0.65529999999999999</v>
-      </c>
-      <c r="H94" s="6"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+      <c r="D97" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G95" s="6">
-        <v>0.79520000000000002</v>
-      </c>
-      <c r="H95" s="6"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="G96" s="6">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="H96" s="6"/>
-    </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G97" s="1"/>
+      <c r="G97" s="6">
+        <v>0.78149999999999997</v>
+      </c>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
-        <v>127</v>
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="G98" s="6">
-        <v>0.73499999999999999</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G98" s="1"/>
       <c r="H98" s="6"/>
     </row>
     <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
-        <v>129</v>
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G100" s="6">
-        <v>0.6169</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G100" s="1"/>
       <c r="H100" s="6"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G101" s="6">
         <v>0.75</v>
       </c>
       <c r="H101" s="6"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>179</v>
+        <v>54</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="G102" s="6">
-        <v>0.65600000000000003</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G103" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>136</v>
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G104" s="6">
-        <v>0.70819999999999994</v>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="8">
+        <v>0.67420000000000002</v>
       </c>
       <c r="H104" s="6"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G105" s="1"/>
+      <c r="G105" s="6">
+        <v>0.75929999999999997</v>
+      </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G106" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="3">
+        <v>0.52090000000000003</v>
+      </c>
       <c r="H106" s="1"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>136</v>
+      <c r="A107" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G107" s="6">
-        <v>0.78149999999999997</v>
+        <v>173</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="8">
+        <v>0.63400000000000001</v>
       </c>
       <c r="H107" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G107" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="IEMOCAP"/>
-        <filter val="IEMOCAP(VoxCeleb1)"/>
-        <filter val="IEMOCAP+Att-HACK"/>
-        <filter val="IEMOCAP+CMUMOSEI+DAIC-WOZ"/>
-        <filter val="IEMOCAP+CMUMOSI"/>
-        <filter val="IEMOCAP+CMU-MOSI"/>
-        <filter val="IEMOCAP+CREMA-D+MSP-Improv"/>
-        <filter val="IEMOCAP+CREMA-D+MSP-Improv+MSP-Podcast"/>
-        <filter val="IEMOCAP+DailyDialog+MELD+EmoryNLP"/>
-        <filter val="IEMOCAP+ESD"/>
-        <filter val="IEMOCAP+MELD"/>
-        <filter val="IEMOCAP+MSP-IMPROV"/>
-        <filter val="IEMOCAP+MSP-Improv+CREMA-D"/>
-        <filter val="IEMOCAP+MSP-Podcast"/>
-        <filter val="IEMOCAP+NNIME"/>
-        <filter val="IEMOCAP+RAVDESS"/>
-        <filter val="IEMOCAP+RAVDESS+EMO-DB"/>
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="语音"/>
+        <filter val="语音+视频"/>
+        <filter val="语音-视频"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G107">
+      <sortCondition ref="A1:A107"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>